<commit_message>
APDL + PRBM Results Added
</commit_message>
<xml_diff>
--- a/Kinematic Analysis/Force_Deflection_Data.xlsx
+++ b/Kinematic Analysis/Force_Deflection_Data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="28" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="36" uniqueCount="4">
   <si>
     <t>Deflection_X_mm</t>
   </si>
@@ -101,7 +101,7 @@
         <v>-0</v>
       </c>
       <c r="B2" s="0">
-        <v>5.6086098084878833e-16</v>
+        <v>1.8732047832379676e-16</v>
       </c>
       <c r="C2" s="0">
         <v>18.000000000000011</v>
@@ -115,13 +115,13 @@
         <v>2.2222222222222285</v>
       </c>
       <c r="B3" s="0">
-        <v>7.1144562793327335</v>
+        <v>8.6741028045005617</v>
       </c>
       <c r="C3" s="0">
-        <v>19.581173274303989</v>
+        <v>19.749328915738147</v>
       </c>
       <c r="D3" s="0">
-        <v>340.41882672569602</v>
+        <v>340.25067108426191</v>
       </c>
     </row>
     <row r="4">
@@ -129,13 +129,13 @@
         <v>4.4444444444444571</v>
       </c>
       <c r="B4" s="0">
-        <v>12.798306435149783</v>
+        <v>15.460914713021179</v>
       </c>
       <c r="C4" s="0">
-        <v>21.048181031337801</v>
+        <v>21.361084002807804</v>
       </c>
       <c r="D4" s="0">
-        <v>338.95181896866222</v>
+        <v>338.63891599719221</v>
       </c>
     </row>
     <row r="5">
@@ -143,13 +143,13 @@
         <v>6.6666666666666572</v>
       </c>
       <c r="B5" s="0">
-        <v>17.487098238379005</v>
+        <v>20.976379169051555</v>
       </c>
       <c r="C5" s="0">
-        <v>22.423471356225814</v>
+        <v>22.864417438491312</v>
       </c>
       <c r="D5" s="0">
-        <v>337.57652864377422</v>
+        <v>337.13558256150867</v>
       </c>
     </row>
     <row r="6">
@@ -157,13 +157,13 @@
         <v>8.8888888888888857</v>
       </c>
       <c r="B6" s="0">
-        <v>21.451122187028215</v>
+        <v>25.587849945264185</v>
       </c>
       <c r="C6" s="0">
-        <v>23.723029429968232</v>
+        <v>24.279515549106414</v>
       </c>
       <c r="D6" s="0">
-        <v>336.27697057003178</v>
+        <v>335.72048445089359</v>
       </c>
     </row>
     <row r="7">
@@ -171,13 +171,13 @@
         <v>11.111111111111114</v>
       </c>
       <c r="B7" s="0">
-        <v>24.868158800643013</v>
+        <v>29.529777375310879</v>
       </c>
       <c r="C7" s="0">
-        <v>24.958715183094913</v>
+        <v>25.621039470848146</v>
       </c>
       <c r="D7" s="0">
-        <v>335.04128481690509</v>
+        <v>334.37896052915187</v>
       </c>
     </row>
     <row r="8">
@@ -185,13 +185,13 @@
         <v>13.333333333333343</v>
       </c>
       <c r="B8" s="0">
-        <v>27.860565817103669</v>
+        <v>32.959746344041726</v>
       </c>
       <c r="C8" s="0">
-        <v>26.139614853007302</v>
+        <v>26.900034517825578</v>
       </c>
       <c r="D8" s="0">
-        <v>333.86038514699271</v>
+        <v>333.09996548217441</v>
       </c>
     </row>
     <row r="9">
@@ -199,13 +199,13 @@
         <v>15.555555555555543</v>
       </c>
       <c r="B9" s="0">
-        <v>30.515677282275821</v>
+        <v>35.988105245180286</v>
       </c>
       <c r="C9" s="0">
-        <v>27.27287163912785</v>
+        <v>28.125066913004545</v>
       </c>
       <c r="D9" s="0">
-        <v>332.72712836087214</v>
+        <v>331.87493308699544</v>
       </c>
     </row>
     <row r="10">
@@ -213,13 +213,13 @@
         <v>17.777777777777771</v>
       </c>
       <c r="B10" s="0">
-        <v>32.89771917579489</v>
+        <v>38.694736190202732</v>
       </c>
       <c r="C10" s="0">
-        <v>28.364221613881725</v>
+        <v>29.302938728976116</v>
       </c>
       <c r="D10" s="0">
-        <v>331.63577838611832</v>
+        <v>330.69706127102393</v>
       </c>
     </row>
     <row r="11">
@@ -227,13 +227,13 @@
         <v>20</v>
       </c>
       <c r="B11" s="0">
-        <v>35.055118457873462</v>
+        <v>41.139080203554784</v>
       </c>
       <c r="C11" s="0">
-        <v>29.418353432253223</v>
+        <v>30.439157851663548</v>
       </c>
       <c r="D11" s="0">
-        <v>330.58164656774682</v>
+        <v>329.56084214833646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>